<commit_message>
forecast parameters adjusted to increase weight of past data in smoothing, because NH vaccinations have step variations that are probably one-time
</commit_message>
<xml_diff>
--- a/vaccinations/data/vaccine capacity.xlsx
+++ b/vaccinations/data/vaccine capacity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aligo/Downloads/FEMA recovery data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aligo/git-repos/FEMA/vaccinations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CA507D-2A33-4046-AC04-76DC4BB09223}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C24F55-F29D-6644-B6F6-77604C2B610C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{BA58EDBF-C5FE-A846-B6BF-204006ECDCEF}"/>
   </bookViews>
@@ -95,10 +95,10 @@
     <t>Source</t>
   </si>
   <si>
-    <t>See 20210222 Vax Sites per State Sources and Assumptions.xlsx</t>
-  </si>
-  <si>
     <t>KV</t>
+  </si>
+  <si>
+    <t>See 2021-03-30 Vax Sites per State.docx</t>
   </si>
 </sst>
 </file>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FAB2862-08EA-3740-A35D-D6B23AB9F9F6}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,7 +509,7 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>104</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -565,7 +565,7 @@
         <v>14</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
         <v>Pharmacy</v>
       </c>
       <c r="D10">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -638,7 +638,7 @@
         <v>Type 1</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>Medical facility</v>
       </c>
       <c r="D16">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>Pharmacy</v>
       </c>
       <c r="D17">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>Type 3</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,7 +788,7 @@
         <v>Type 4</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -938,7 +938,7 @@
         <v>Pharmacy</v>
       </c>
       <c r="D31">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -968,7 +968,7 @@
         <v>Type 2</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -998,8 +998,7 @@
         <v>Type 4</v>
       </c>
       <c r="D35">
-        <f>ROUND(D29/2,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1044,7 +1043,7 @@
         <v>Pharmacy</v>
       </c>
       <c r="D38">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1880,7 +1879,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1892,10 +1891,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>